<commit_message>
GM-233 add product select in licenses import, update licenses importer to use product in import modal
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>product_id</t>
   </si>
   <si>
     <t>quantity</t>
@@ -396,23 +393,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GM-1068 eliminate quantity columns from license upload template which is not used anymore
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -393,20 +390,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>